<commit_message>
Upload dos novos assets
</commit_message>
<xml_diff>
--- a/Assets/BaseCalculos.xlsx
+++ b/Assets/BaseCalculos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jogos Unity\StoneJungleCityV2\StoneJungleCity\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5676D4E6-0173-4F6B-8569-050E0F92EA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C370724-668C-4727-86FD-F98A42806334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{83CD1AD5-219E-4A39-8021-D8F43162BD44}"/>
+    <workbookView xWindow="2535" yWindow="0" windowWidth="18885" windowHeight="12585" activeTab="1" xr2:uid="{83CD1AD5-219E-4A39-8021-D8F43162BD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculo Level por XP" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Level</t>
   </si>
@@ -174,6 +174,33 @@
   </si>
   <si>
     <t>Bolsa de Valores</t>
+  </si>
+  <si>
+    <t>Posto de Gasolina</t>
+  </si>
+  <si>
+    <t>Comercial Trade</t>
+  </si>
+  <si>
+    <t>Contabil</t>
+  </si>
+  <si>
+    <t>BoateLux</t>
+  </si>
+  <si>
+    <t>Comercial Stone</t>
+  </si>
+  <si>
+    <t>Emissora</t>
+  </si>
+  <si>
+    <t>Hotel Stone</t>
+  </si>
+  <si>
+    <t>Comercial Cosmético</t>
+  </si>
+  <si>
+    <t>Estúdio Indie</t>
   </si>
 </sst>
 </file>
@@ -297,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -374,6 +401,15 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -388,12 +424,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -740,7 +770,7 @@
       <c r="B2" s="1">
         <v>60</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
     </row>
@@ -752,7 +782,7 @@
         <f>B2*1.2</f>
         <v>72</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -762,7 +792,7 @@
         <f t="shared" ref="B4:B21" si="0">B3*1.2</f>
         <v>86.399999999999991</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -772,7 +802,7 @@
         <f t="shared" si="0"/>
         <v>103.67999999999999</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -782,7 +812,7 @@
         <f t="shared" si="0"/>
         <v>124.41599999999998</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -792,7 +822,7 @@
         <f t="shared" si="0"/>
         <v>149.29919999999998</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="31"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -802,7 +832,7 @@
         <f t="shared" si="0"/>
         <v>179.15903999999998</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -812,7 +842,7 @@
         <f t="shared" si="0"/>
         <v>214.99084799999997</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="31"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -822,7 +852,7 @@
         <f t="shared" si="0"/>
         <v>257.98901759999995</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="31"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -832,7 +862,7 @@
         <f t="shared" si="0"/>
         <v>309.58682111999991</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -842,7 +872,7 @@
         <f t="shared" si="0"/>
         <v>371.50418534399989</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -852,7 +882,7 @@
         <f t="shared" si="0"/>
         <v>445.80502241279987</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -862,7 +892,7 @@
         <f t="shared" si="0"/>
         <v>534.96602689535985</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -872,7 +902,7 @@
         <f t="shared" si="0"/>
         <v>641.95923227443177</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -882,7 +912,7 @@
         <f t="shared" si="0"/>
         <v>770.35107872931815</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="31"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -892,7 +922,7 @@
         <f t="shared" si="0"/>
         <v>924.42129447518175</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="31"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -902,7 +932,7 @@
         <f t="shared" si="0"/>
         <v>1109.3055533702181</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -912,7 +942,7 @@
         <f t="shared" si="0"/>
         <v>1331.1666640442618</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -922,7 +952,7 @@
         <f t="shared" si="0"/>
         <v>1597.3999968531141</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="31"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -932,7 +962,7 @@
         <f t="shared" si="0"/>
         <v>1916.8799962237367</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -942,7 +972,7 @@
         <f>B21*1.3</f>
         <v>2491.9439950908577</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="31" t="s">
         <v>3</v>
       </c>
     </row>
@@ -954,7 +984,7 @@
         <f t="shared" ref="B23:B36" si="1">B22*1.5</f>
         <v>3737.9159926362863</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -964,7 +994,7 @@
         <f t="shared" si="1"/>
         <v>5606.8739889544295</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -974,7 +1004,7 @@
         <f t="shared" si="1"/>
         <v>8410.3109834316438</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
@@ -984,7 +1014,7 @@
         <f t="shared" si="1"/>
         <v>12615.466475147467</v>
       </c>
-      <c r="C26" s="28"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -994,7 +1024,7 @@
         <f t="shared" si="1"/>
         <v>18923.199712721202</v>
       </c>
-      <c r="C27" s="28"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -1004,7 +1034,7 @@
         <f t="shared" si="1"/>
         <v>28384.799569081802</v>
       </c>
-      <c r="C28" s="28"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
@@ -1014,7 +1044,7 @@
         <f t="shared" si="1"/>
         <v>42577.199353622702</v>
       </c>
-      <c r="C29" s="28"/>
+      <c r="C29" s="31"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -1024,7 +1054,7 @@
         <f t="shared" si="1"/>
         <v>63865.799030434049</v>
       </c>
-      <c r="C30" s="28"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
@@ -1034,7 +1064,7 @@
         <f t="shared" si="1"/>
         <v>95798.698545651074</v>
       </c>
-      <c r="C31" s="28"/>
+      <c r="C31" s="31"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
@@ -1044,7 +1074,7 @@
         <f t="shared" si="1"/>
         <v>143698.04781847663</v>
       </c>
-      <c r="C32" s="28"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
@@ -1054,7 +1084,7 @@
         <f t="shared" si="1"/>
         <v>215547.07172771494</v>
       </c>
-      <c r="C33" s="28"/>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
@@ -1064,7 +1094,7 @@
         <f t="shared" si="1"/>
         <v>323320.60759157239</v>
       </c>
-      <c r="C34" s="28"/>
+      <c r="C34" s="31"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
@@ -1074,7 +1104,7 @@
         <f t="shared" si="1"/>
         <v>484980.91138735856</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="31"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -1084,7 +1114,7 @@
         <f t="shared" si="1"/>
         <v>727471.36708103784</v>
       </c>
-      <c r="C36" s="28"/>
+      <c r="C36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1131,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A59586-0C0B-4140-93D4-3BF2EBFC0FC3}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,39 +1171,39 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="H1" s="30" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="O1" s="31" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="O1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="V1" s="32" t="s">
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="V1" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1593,7 +1623,7 @@
       <c r="D9" s="9">
         <v>7</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="28">
         <v>3</v>
       </c>
       <c r="H9" s="11">
@@ -1649,7 +1679,7 @@
         <f t="shared" si="1"/>
         <v>8.0500000000000007</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="28">
         <v>3</v>
       </c>
       <c r="H10" s="11">
@@ -1678,7 +1708,7 @@
       <c r="Q10" s="20">
         <v>2800</v>
       </c>
-      <c r="R10" s="34">
+      <c r="R10" s="29">
         <v>520</v>
       </c>
       <c r="S10" s="21">
@@ -1705,7 +1735,7 @@
       <c r="D11" s="9">
         <v>15</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="28">
         <v>5</v>
       </c>
       <c r="H11" s="11">
@@ -1761,7 +1791,7 @@
       <c r="D12" s="9">
         <v>30</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="28">
         <v>10</v>
       </c>
       <c r="H12" s="11">
@@ -1783,10 +1813,18 @@
       <c r="O12" s="17">
         <v>70</v>
       </c>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="21"/>
+      <c r="P12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>10500</v>
+      </c>
+      <c r="R12" s="20">
+        <v>1800</v>
+      </c>
+      <c r="S12" s="21">
+        <v>18</v>
+      </c>
       <c r="V12" s="23">
         <v>100</v>
       </c>
@@ -1809,7 +1847,7 @@
       <c r="D13" s="9">
         <v>125</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="28">
         <v>6</v>
       </c>
       <c r="H13" s="11">
@@ -1822,10 +1860,18 @@
       <c r="O13" s="17">
         <v>71</v>
       </c>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="21"/>
+      <c r="P13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q13" s="20">
+        <v>8600</v>
+      </c>
+      <c r="R13" s="20">
+        <v>780</v>
+      </c>
+      <c r="S13" s="21">
+        <v>10</v>
+      </c>
       <c r="V13" s="23">
         <v>101</v>
       </c>
@@ -1849,7 +1895,7 @@
         <f t="shared" si="1"/>
         <v>143.75</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="11">
@@ -1862,10 +1908,18 @@
       <c r="O14" s="17">
         <v>72</v>
       </c>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="21"/>
+      <c r="P14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q14" s="20">
+        <v>4600</v>
+      </c>
+      <c r="R14" s="20">
+        <v>520</v>
+      </c>
+      <c r="S14" s="21">
+        <v>8</v>
+      </c>
       <c r="V14" s="23">
         <v>102</v>
       </c>
@@ -1889,7 +1943,7 @@
         <f t="shared" si="1"/>
         <v>165.3125</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="11">
@@ -1902,10 +1956,18 @@
       <c r="O15" s="17">
         <v>73</v>
       </c>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="21"/>
+      <c r="P15" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q15" s="20">
+        <v>16500</v>
+      </c>
+      <c r="R15" s="20">
+        <v>1920</v>
+      </c>
+      <c r="S15" s="21">
+        <v>14</v>
+      </c>
       <c r="V15" s="23">
         <v>103</v>
       </c>
@@ -1929,7 +1991,7 @@
         <f t="shared" si="1"/>
         <v>190.109375</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="11">
@@ -1942,10 +2004,18 @@
       <c r="O16" s="17">
         <v>74</v>
       </c>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="21"/>
+      <c r="P16" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="20">
+        <v>9600</v>
+      </c>
+      <c r="R16" s="20">
+        <v>1110</v>
+      </c>
+      <c r="S16" s="21">
+        <v>14</v>
+      </c>
       <c r="V16" s="23">
         <v>104</v>
       </c>
@@ -1969,7 +2039,7 @@
         <f t="shared" si="1"/>
         <v>218.62578124999999</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="11">
@@ -1982,10 +2052,18 @@
       <c r="O17" s="17">
         <v>75</v>
       </c>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="21"/>
+      <c r="P17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>16800</v>
+      </c>
+      <c r="R17" s="20">
+        <v>2100</v>
+      </c>
+      <c r="S17" s="21">
+        <v>18</v>
+      </c>
       <c r="V17" s="23">
         <v>105</v>
       </c>
@@ -2009,7 +2087,7 @@
         <f t="shared" si="1"/>
         <v>251.41964843749997</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="11">
@@ -2022,10 +2100,18 @@
       <c r="O18" s="17">
         <v>76</v>
       </c>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="21"/>
+      <c r="P18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>12500</v>
+      </c>
+      <c r="R18" s="20">
+        <v>1280</v>
+      </c>
+      <c r="S18" s="30">
+        <v>16</v>
+      </c>
       <c r="V18" s="23">
         <v>106</v>
       </c>
@@ -2049,7 +2135,7 @@
         <f t="shared" si="1"/>
         <v>289.13259570312499</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="11">
@@ -2062,10 +2148,18 @@
       <c r="O19" s="17">
         <v>77</v>
       </c>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="21"/>
+      <c r="P19" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>9400</v>
+      </c>
+      <c r="R19" s="20">
+        <v>980</v>
+      </c>
+      <c r="S19" s="21">
+        <v>10</v>
+      </c>
       <c r="V19" s="23">
         <v>107</v>
       </c>
@@ -2089,7 +2183,7 @@
         <f t="shared" si="1"/>
         <v>332.50248505859372</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="11">
@@ -2102,10 +2196,18 @@
       <c r="O20" s="17">
         <v>78</v>
       </c>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="21"/>
+      <c r="P20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>16000</v>
+      </c>
+      <c r="R20" s="20">
+        <v>3500</v>
+      </c>
+      <c r="S20" s="21">
+        <v>16</v>
+      </c>
       <c r="V20" s="23">
         <v>108</v>
       </c>

</xml_diff>